<commit_message>
Implemented passes per second and time of possesion percentages
</commit_message>
<xml_diff>
--- a/final_report/all_games.xlsx
+++ b/final_report/all_games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evankim/Desktop/Projects/Water-Polo-Analytics/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1417CD6-260E-EF48-9209-471A68AC9E2A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4F6840-F931-024E-9F55-8A757470CECA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="868">
   <si>
     <t>Number of Passes</t>
   </si>
@@ -2679,11 +2679,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2988,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="O126" sqref="O126"/>
+    <sheetView tabSelected="1" topLeftCell="D156" workbookViewId="0">
+      <selection activeCell="O164" sqref="O164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18265,11 +18266,11 @@
       <c r="S184">
         <v>4</v>
       </c>
-      <c r="T184" t="s">
-        <v>259</v>
-      </c>
-      <c r="U184" t="s">
-        <v>288</v>
+      <c r="T184" s="2">
+        <v>0.10277777777777779</v>
+      </c>
+      <c r="U184" s="2">
+        <v>8.819444444444445E-2</v>
       </c>
       <c r="V184">
         <v>2</v>

</xml_diff>

<commit_message>
Fixed bucketing of passes per second
</commit_message>
<xml_diff>
--- a/final_report/all_games.xlsx
+++ b/final_report/all_games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evankim/Desktop/Projects/Water-Polo-Analytics/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4F6840-F931-024E-9F55-8A757470CECA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE62A2B-27C3-3442-A667-0EE02D83E8F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2989,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D156" workbookViewId="0">
-      <selection activeCell="O164" sqref="O164"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10219,7 +10219,7 @@
         <v>75</v>
       </c>
       <c r="L87" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="M87">
         <v>4</v>
@@ -15273,7 +15273,7 @@
         <v>53</v>
       </c>
       <c r="L148" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="M148">
         <v>1</v>
@@ -16553,7 +16553,7 @@
         <v>75</v>
       </c>
       <c r="L164" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="M164">
         <v>4</v>
@@ -19449,7 +19449,7 @@
         <v>53</v>
       </c>
       <c r="L199" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="M199">
         <v>4</v>
@@ -21329,7 +21329,7 @@
         <v>53</v>
       </c>
       <c r="L221" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="M221">
         <v>4</v>

</xml_diff>

<commit_message>
Fixed data mid -> middle
</commit_message>
<xml_diff>
--- a/final_report/all_games.xlsx
+++ b/final_report/all_games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evankim/Desktop/Projects/Water-Polo-Analytics/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE62A2B-27C3-3442-A667-0EE02D83E8F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0C787B-7A9A-354A-89A2-13A18D67BA38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2989,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6753,7 +6753,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>247</v>
+        <v>75</v>
       </c>
       <c r="L46" t="s">
         <v>96</v>
@@ -7951,7 +7951,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="s">
-        <v>247</v>
+        <v>75</v>
       </c>
       <c r="L60" t="s">
         <v>30</v>
@@ -8808,7 +8808,7 @@
         <v>0</v>
       </c>
       <c r="K70" t="s">
-        <v>247</v>
+        <v>75</v>
       </c>
       <c r="L70" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Added percentages based on result of game
</commit_message>
<xml_diff>
--- a/final_report/all_games.xlsx
+++ b/final_report/all_games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evankim/Desktop/Projects/Water-Polo-Analytics/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0C787B-7A9A-354A-89A2-13A18D67BA38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8FF34A-637F-1F40-B73C-4176086AD695}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2989,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="Q93" sqref="Q93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>